<commit_message>
working on authentication and responsive front-end
</commit_message>
<xml_diff>
--- a/Vocab.xlsx
+++ b/Vocab.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Paulina foldery\Python projects\NorwegianApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PaulinaFoldery\MyProjects\NorwegianApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E72F84A-EA89-4749-BC89-CA9BC858EDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3058F8-FBEF-41F8-8199-3FB81DB68C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C2818DB8-A898-4F8E-B725-2FA7E8E68A7F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2818DB8-A898-4F8E-B725-2FA7E8E68A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="nowe" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>norweski</t>
   </si>
@@ -568,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C546D52-F6A8-413C-95DC-E0FB1F357EF1}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,50 +947,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6797B09D-AC90-452B-B976-25DE1883668D}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>